<commit_message>
Fix: Typo & Update Excel
</commit_message>
<xml_diff>
--- a/Build/Signal_Lost_Chapters.xlsx
+++ b/Build/Signal_Lost_Chapters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developpement\Games\Visual Studio 2026\C++\Signal_Lost\Signal_Lost\Build\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4476118-A620-402F-98D6-A3D8FEEF83A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCD761B-31E6-4BE2-8F52-47A4B68044EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="528" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="528" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chapters_Header" sheetId="3" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="642">
   <si>
     <t>Chapter Name</t>
   </si>
@@ -841,12 +841,6 @@
 I know which one it is since I've got the same memories as you, eheh![Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>Ahahah![Wait=500] That's tru-.[Wait=500][Space=2]
-[Color=Yellow]We have to go.[Color=White][Wait=500][Space=2]
-O-Oh...[Wait=500] Well, I guess it's a goodbye.[Wait=500][Space=2]
-I really hope to see you again.[Wait=500] Until then, believe in yourself.[Wait=500] I know we're great people.[Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>[Choice1=[NextScene=3][Content=Small?]]
 [Choice2=[NextScene=4][Content=Well-preserved?]]</t>
   </si>
@@ -1010,13 +1004,6 @@
 ...[Wait=500] There's clearly a fuse missing here...[Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>[Color=Gray]*B[Beep=True]UZZ*[Color=White]...[Wait=500] That wasn't a reassuring sou-.[Wait=500][Space=2]
-[Color=Red]PASSWORD INCORRECT.[Wait=500] ENGAGING ANTI-INTRUDER PROTOCOL.[Color=White][Wait=500][Space=2]
-...W-[Wait=500] What?[Wait=500] What does that even mean?[Wait=500][Space=2]
-[Color=Gray]*Cough*[Color=White]...[Wait=500] You gave me the wrong letter![Wait=500][Space=2]
-[Color=Gray]*Cough*[Color=White]...[Wait=500] Why is everything get-[Color=Gray]*Cough*[Color=White]...[Wait=500] getting blurry?[Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>[Color=Gray]*Cough*[Color=White]... [Color=Gray]*COUGH*[Color=White]...[Wait=500][Space=2]
 I c...[Wait=500] [Color=Gray]*Cough*[Color=White]...[Wait=500] I can't breathe![Wait=500][Space=2]
 [Color=Gray]*Cough*[Color=White]... [Color=Gray]*COUGH*[Color=White]... [Color=Gray]*COUGH*[Color=White]...[Wait=500][Space=2]
@@ -1046,12 +1033,6 @@
   <si>
     <t>Yeah, as if you could pretend that![Wait=500][Space=2]
 Anyway, let's focus on the most important question.[Wait=500] WHO WAS THAT?[Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>[Color=Gray]*Footsteps*[Color=White]...[Wait=500] It's getting closer![Wait=500][Space=2]
-[Color=Gray]*SLAM*[Color=White]...[Wait=500][Space=2]
-I locked myself inside a room...[Wait=500] I think I'm safe n-.[Wait=500][Space=2]
-[Color=Yellow]It's useless to hide, you know?[Wait=500] I know where you are at all times.[Color=White][Wait=500][Space=2]</t>
   </si>
   <si>
     <t>N-NO![Wait=500] I WON'T FOLLOW HIM![Wait=500][Space=2]
@@ -1879,22 +1860,7 @@
 Too bad I can't speak that language, though.[Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>I thought the same thing...[Wait=500][Space=2]
-I'm not here to appreciate the beauty of handmade art.[Wait=500][Space=2]
-I'm here to GET OFF THIS ISLAND![Wait=500] FUCK YOU, ART![Wait=500][Space=2]
-[Color=Gray]*CRACK*[Color=White]...[Wait=500][Space=2]
-Shit, I didn't know kicking a statue could dislocate its leg-.[Wait=500][Space=2]
-[Color=Gray]*RUMBLE*[Color=White]...[Wait=500][Space=2]
-Huh?[Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>[Choice1=[NextScene=32][Content=What's going on?]]</t>
-  </si>
-  <si>
-    <t>I-I don't know. The ground shook for a second...[Wait=500][Space=2]
-Wait...[Wait=500] What's tha-.[Wait=500][Space=2]
-...Did a motherfucking door just appear at the back of the museum?![Wait=500][Space=2]
-Did I really activate a mechanism at random because of my rage?[Wait=500][Space=2]</t>
   </si>
   <si>
     <t>I don't know, but I'm too curious not to see what this damn door is all about![Wait=500][Space=2]
@@ -2571,20 +2537,6 @@
 Tell me where to go.[Wait=500][Space=2]</t>
   </si>
   <si>
-    <t>Left it is![Wait=500][Space=2]
-Well tha-.[Wait=500][Space=2]
-Fuck.[Wait=500] I heard something behind me.[Wait=500][Space=2]
-Oh no...[Wait=500] OH SHIT SHIT SHIT IT'S RUNNING TOWARDS ME!!![Wait=500][Space=2]
-WHERE DO I GO?! QUICK!!![Wait=500][Space=2]</t>
-  </si>
-  <si>
-    <t>Are you sure it's this way?![Wait=500][Space=2]
-There's something strange about this pla-[Color=Gray]*Cracking noises*[Color=White]...[Wait=500][Space=2]
-...[Wait=500] Don't tell me the ground is-.[Wait=500][Space=2]
-[Color=Gray]*COLLAPSING RUCKUS*[Color=White]...[Wait=500][Space=2]
-WOAAAAAAH SHIIII-[Color=Gray]*THUD*[Color=White]...[Wait=500][Space=2]</t>
-  </si>
-  <si>
     <t>[Choice1=[NextScene=67][Content=Hey! Tell me you're still alive!]]</t>
   </si>
   <si>
@@ -3062,6 +3014,263 @@
 [Color=Yellow]You won't be here to witness it anyway.[Color=White][Wait=500][Space=2]
 Don't tell me you-[Color=Gray]*BANG*[Color=White]...[Wait=500][Space=2]
 ...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>With how much all of this looks like a setup, I might find the fuse there.[Wait=500][Space=2]
+I just don't get why whoever is keeping me in this place left a working phone back in the supermarket.[Wait=500][Space=2]
+I'm just playing their game at this point.[Wait=500][Space=2]
+[Color=Gray]*Footsteps*[Color=White]...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Yeah.[Wait=500] Of all places, the factory seems like the place I could find answers and the key to my escape.[Wait=500][Space=2]
+I'll go there if I can.[Wait=500] Let's go.[Wait=500][Space=2]
+[Color=Gray]*Footsteps*[Color=White]...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>...[Wait=500] I hope I can find the fuse, why are you asking?[Wait=500][Space=2]
+[Color=Gray]*Footsteps*[Color=White]...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>You- I mean, you know-...[Wait=500] I get it.[Wait=500][Space=2]
+It's hard to handle some random person calling you for seemingly no reason.[Wait=500][Space=2]
+...[Wait=500][Space=2]
+But thanks for admitting that, I already feel safer if you're able to show a bit of self-awareness.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=2][NextSceneNoTrust=3][TrustNeed=50][Content=What exactly do you mean by key?]]
+[Choice2=[NextScene=9][NextSceneNoTrust=10][TrustNeed=50][Content=If you can? Would there be anything preventing you?]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=8][Content=That's a pain of a situation for sure.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=4][Content=Are you... alright?]]
+[Choice2=[NextScene=7][Content=Of course. Just making sure.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=5][TrustAdd=25][Content=It's my fault, I behaved like an idiot.]]
+[Choice2=[NextScene=7][Content=You're right, let's both calm down and work together.]]
+[Choice3=[NextScene=7][Content=I'm sorry, I wasn't expecting a call like that.]]</t>
+  </si>
+  <si>
+    <t>[Choice1=[NextScene=6][Content=We're cool then!]]</t>
+  </si>
+  <si>
+    <t>We are.[Wait=500][Space=2]
+...[Wait=500][Space=2]
+I've arrived to the entrance, but I have to get through a fence.[Wait=500][Space=2]
+It seems really fragile, so getting rid of it wouldn't be that hard.[Wait=500] That thing's already quite damaged.[Wait=500][Space=2]
+...[Wait=500][Space=2]
+Or I could go around, there's no reason for a building like this not to have some kind of backdoor.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Alright...[Wait=500][Space=2]
+...[Wait=500][Space=2]
+There's a metal fence around the entrance.[Wait=500][Space=2]
+I should be able to push it, but going around and finding another entrance might be easier.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Kind of...[Wait=500] Yeah.[Wait=500][Space=2]
+...[Wait=500][Space=2]
+I got closer to the building, enough to realise the entrance's blocked by a fence.[Wait=500][Space=2]
+It looks brittle enough, but getting around might also be easier.[Wait=500][Space=2]
+It only seems to block the main entrance.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>There seem to be a fence in front of the main entrance.[Wait=500][Space=2]
+I probably could get around and find another way to enter.[Wait=500][Space=2]
+But from this distance it looks really thin and rusted.[Wait=500][Space=2]
+I think pushing it down and getting over would prove quite easy.[Wait=500][Space=2]
+What do you think?[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Do you expect something to block me?[Wait=500] Why would you ask me that?[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>I got myself a smart one, uh?[Wait=500][Space=2]
+I'm being conditional, cause there's a fence surrounding the entrance.[Wait=500][Space=2]
+Either have to get around or through it.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>I-[Wait=500] I get it.[Wait=500][Space=2]
+It's good you're able to put yourself in my place a bit.[Wait=500] Thanks for acknowledging it.[Wait=500][Space=2]
+I'm starting to feel a bit more hopeful about getting out of here if you're on my side.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>I'm getting there.[Wait=500] But I can already see the place's protected by a fence.[Wait=500][Space=2]
+It isn't a big deal, I could probably find another entrance.[Wait=500][Space=2]
+[Color=Gray]*Footsteps*[Color=White]...[Wait=500][Space=2]
+The metal looks brittle. I probably could bend it down and get over it.[Wait=500][Space=2]
+What do you think?[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Hm-[Wait=500] Anyways, there's a fence blocking the way to the main entrance.[Wait=500][Space=2]
+I can either try and get through or go around.[Wait=500][Space=2]
+It looks weak enough to be bent, but this kind of buildings tend to have backdoors.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Yeah. The main entrance might be trapped, I'd rather find another way.[Wait=500][Space=2]
+[Color=Gray]*Footsteps*[Color=White]...[Wait=500][Space=2]
+Thinking outside the box might be the way to avoid some of the-[Wait=500] psycho keeping me here.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Good to know we're on the same line.[Wait=500][Space=2]
+...[Wait=500][Space=2]
+I know it sounds weird, but...[Wait=500] I really like the slight breeze on this island.[Wait=500][Space=2]
+If it wasn't covered in trash and dull concrete, it'd be almost habitable.[Wait=500][Space=2]
+I almost regret not going for a walk in the zoo.[Wait=500][Space=2]
+But I really need to find food and I'm not about eating a raw giraffe.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>...[Wait=500] No need to make me doubt...[Wait=500][Space=2]
+If that bastard really wants me to die I'm screwed anyways. Might as well minimize the risk.[Wait=500][Space=2]
+...[Wait=500][Space=2]
+Who knows...[Wait=500] He might be an idiot.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Talking about the zoo, guess what.[Wait=500] It's awfully close to this place.[Wait=500][Space=2]
+I can see the inside of the enclosures from there.[Wait=500][Space=2]
+Whoever designed this city should be fired.[Wait=500] Or even set on fire.[Wait=500][Space=2]
+Because I'm stuck inside their shittily designed city.[Wait=500][Space=2]
+That prick.[Wait=500][Space=2]
+[Color=Magenta][Beep=True][Color=Gray]*Distorted chuckle*[Color=White]...[Wait=500][Space=2]
+[Color=Magenta][Beep=True]YoU'[Wait=500][Beep=True]rE bEt[Wait=500][Beep=True]tEr hErE[Wait=500][Beep=True]  wItH mE[Wait=500][Beep=True]  tHaN aLo[Wait=500][Beep=True]nE iN[Wait=500][Beep=True]  tHe zOo.[Color=White][Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Wouldn't be trying to defend them, would we?[Wait=500][Space=2]
+Errm-[Wait=500] Anyways.[Wait=500][Space=2]
+Didn't realize the zoo was that close to the factory before.[Wait=500] Civil engineering failed some.[Wait=500][Space=2]
+[Color=Magenta][Beep=True]DaN[Wait=500][Beep=True]gErOuS[Wait=500][Beep=True]  pLa[Wait=500][Beep=True]cE.[Wait=500][Beep=True]  ExpEr[Wait=500][Beep=True]iMeNtS.[Color=White][Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Empty drums, debris, nothing but the usual shit.[Wait=500][Space=2]
+Nowhere else to go, you see, so for now I'll keep looking.[Wait=500][Space=2]
+Stressed out and hungry I feel, still haven't got anything to eat.[Wait=500][Space=2]
+I could really use oat meal, or anything that would get me going.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>You're-...[Wait=500][Space=2]
+There's something written on the wall.[Wait=500][Space=2]
+...[Wait=500][Space=2]
+Please don't be scary.[Wait=500][Space=2]
+...[Wait=500][Space=2]
+Oh god.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>M-[Wait=500] Me?[Wait=500] As I've said before I-...[Wait=500][Space=2]
+[Color=Magenta][Beep=True]OnE[Wait=500][Beep=True]  oF tHe[Wait=500][Beep=True]  pReVi[Wait=500][Beep=True]oUs.[Color=White][Wait=500] [Color=Gray]*Static*[Color=White]...[Wait=500][Space=2]
+[Color=Magenta][Beep=True]I'M[Wait=500][Beep=True]  hErE tO[Wait=500][Beep=True]  hElP yOu[Wait=500][Beep=True].  I'M aBlE[Wait=500][Beep=True]  tO cOmMu[Wait=500][Beep=True]nIcAtE tHrOuGh[Wait=500][Beep=True]  tHe dEsA[Wait=500][Beep=True]fEcTeD cOnTrOl.[Color=White][Wait=500][Space=2]
+[Color=Gray]*Static*[Color=White]...[Wait=500][Space=2]
+[Color=Magenta][Beep=True]SuR[Wait=500]viVoR[Wait=500][Beep=True],  i’M tRy[Wait=500][Beep=True]iNg tO gEt[Wait=500][Beep=True]  oThErS oUt[Wait=500][Beep=True]  oF hIs[Wait=500][Beep=True]  tRaPs.[Color=White][Wait=500][Space=2]
+Once again, I do NOT know why I'm here nor about any kind of experiments, just help me, alright?[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>What?[Wait=500] Who are you talking to?[Wait=500] You're really starting to freak me out.[Wait=500][Space=2]
+[Color=Magenta][Beep=True]CaN[Wait=500][Beep=True]’t sAy[Wait=500][Beep=True]  mOrE[Wait=500][Beep=True].  cOnNeC[Wait=500][Beep=True]tIoN  uNsTa[Wait=500][Beep=True]bLe[Wait=500][Beep=True].  yOu’Ll[Wait=500][Beep=True]  gEt cLo[Wait=500][Beep=True]sEr.[Color=White][Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Of course I'm going to worry!!![Wait=500][Space=2]
+You're giving me no explanation after saying shit about some experiment. Are there more people with you?[Wait=500][Space=2]
+...[Wait=500][Space=2]
+You're always alternating between reinsuring and cryptic, talking to the fucking voices now![Wait=500][Space=2]
+Am-[Wait=500] Am I a game to you?[Wait=500] Are you going to fucking tell?![Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>And...[Wait=500] You're just gonna say that now?[Wait=500][Space=2]
+Uh...[Wait=500] Nevermind. I'm not even gonna ask anymore.[Wait=500][Space=2]
+.[Wait=500].[Wait=500].[Wait=500][Space=2]
+But should we reaaally trust them?[Wait=500][Space=2]
+I mean, why would anyone other than the person behind all of this try to talk to you.[Wait=500][Space=2]
+And why can't I hear them?[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Which means...[Wait=500] They're on the island.[Wait=500][Space=2]
+Great.[Wait=500][Space=2]
+That either means a helping hand... or extra danger.[Wait=500][Space=2]
+As if all of this needed more complexity.[Wait=500][Space=2]
+So they're going to help you guide me if I understood well.[Wait=500][Space=2]
+Doesn't sound like a trap.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Yeah...[Wait=500] I know.[Wait=500][Space=2]
+Let's just think positively![Wait=500] Everything's...[Wait=500] Fine.[Wait=500][Space=2]
+New hope.[Wait=500] Island friend.[Wait=500] Good news aaall around.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Uuh-[Wait=500] Sure...[Wait=500][Space=2]
+...[Wait=500][Space=2]
+I'll-...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Of course.[Wait=500][Space=2]
+Let's just start m-...[Wait=500][Space=2]
+...[Wait=500][Space=2]
+Writings.[Wait=500][Space=2]
+Writings on the wall.[Wait=500] Please.[Wait=500] Why?[Wait=500][Space=2]
+Oh no, don't tell me these are creepy letters-...[Wait=500][Space=2]
+On the wall.[Wait=500] I'm so sick.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Left it is![Wait=500][Space=2]
+Well tha-...[Wait=500][Space=2]
+Fuck.[Wait=500] I heard something behind me.[Wait=500][Space=2]
+Oh no...[Wait=500] OH SHIT SHIT SHIT IT'S RUNNING TOWARDS ME!!![Wait=500][Space=2]
+WHERE DO I GO?! QUICK!!![Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Are you sure it's this way?![Wait=500][Space=2]
+There's something strange about this pla-[Color=Gray]*Cracking noises*[Color=White]...[Wait=500][Space=2]
+...[Wait=500] Don't tell me the ground is-...[Wait=500][Space=2]
+[Color=Gray]*COLLAPSING RUCKUS*[Color=White]...[Wait=500][Space=2]
+WOAAAAAAH SHIIII-[Color=Gray]*THUD*[Color=White]...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>I thought the same thing...[Wait=500][Space=2]
+I'm not here to appreciate the beauty of handmade art.[Wait=500][Space=2]
+I'm here to GET OFF THIS ISLAND![Wait=500] FUCK YOU, ART![Wait=500][Space=2]
+[Color=Gray]*CRACK*[Color=White]...[Wait=500][Space=2]
+Shit, I didn't know kicking a statue could dislocate its leg-...[Wait=500][Space=2]
+[Color=Gray]*RUMBLE*[Color=White]...[Wait=500][Space=2]
+Huh?[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>I-I don't know. The ground shook for a second...[Wait=500][Space=2]
+Wait...[Wait=500] What's tha-...[Wait=500][Space=2]
+...Did a motherfucking door just appear at the back of the museum?![Wait=500][Space=2]
+Did I really activate a mechanism at random because of my rage?[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>[Color=Gray]*B[Beep=True]UZZ*[Color=White]...[Wait=500] That wasn't a reassuring sou-...[Wait=500][Space=2]
+[Color=Red]PASSWORD INCORRECT.[Wait=500] ENGAGING ANTI-INTRUDER PROTOCOL.[Color=White][Wait=500][Space=2]
+...W-[Wait=500] What?[Wait=500] What does that even mean?[Wait=500][Space=2]
+[Color=Gray]*Cough*[Color=White]...[Wait=500] You gave me the wrong letter![Wait=500][Space=2]
+[Color=Gray]*Cough*[Color=White]...[Wait=500] Why is everything get-[Color=Gray]*Cough*[Color=White]...[Wait=500] getting blurry?[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>[Color=Gray]*Footsteps*[Color=White]...[Wait=500] It's getting closer![Wait=500][Space=2]
+[Color=Gray]*SLAM*[Color=White]...[Wait=500][Space=2]
+I locked myself inside a room...[Wait=500] I think I'm safe n-...[Wait=500][Space=2]
+[Color=Yellow]It's useless to hide, you know?[Wait=500] I know where you are at all times.[Color=White][Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Ahahah![Wait=500] That's tru-...[Wait=500][Space=2]
+[Color=Yellow]We have to go.[Color=White][Wait=500][Space=2]
+O-Oh...[Wait=500] Well, I guess it's a goodbye.[Wait=500][Space=2]
+I really hope to see you again.[Wait=500] Until then, believe in yourself.[Wait=500] I know we're great people.[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>I...[Wait=500] I'm just really stressed-...[Wait=500][Space=2]
+...[Wait=500][Space=2]
+Listen, I might have found this phone but I don't feel like you're here to help...[Wait=500][Space=2]
+I don't know, you've got to put yourself in my place a bit...[Wait=500][Space=2]
+[Color=Gray]*Footsteps*[Color=White]...[Wait=500][Space=2]</t>
+  </si>
+  <si>
+    <t>Oh-[Wait=500] Yeah...[Wait=500][Space=2]
+...[Wait=500][Space=2]
+I expected to feel better with someone else on the other end of the phone...[Wait=500] But I-...[Wait=500][Space=2]
+You know...[Wait=500] It's hard...[Wait=500][Space=2]
+[Color=Gray]*Footsteps*[Color=White]...[Wait=500][Space=2]</t>
   </si>
 </sst>
 </file>
@@ -5579,7 +5788,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C2" s="12">
         <v>4</v>
@@ -5695,7 +5904,7 @@
   <sheetPr codeName="Feuil2"/>
   <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="45" zoomScaleNormal="45" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -5717,7 +5926,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>9</v>
@@ -5729,7 +5938,7 @@
         <v>11</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="400.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5776,7 +5985,7 @@
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="8" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>10</v>
@@ -5839,10 +6048,10 @@
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="8" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="G5" s="23" t="str">
         <f t="shared" si="0"/>
@@ -5866,7 +6075,7 @@
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="8" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>17</v>
@@ -5895,7 +6104,7 @@
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="8" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>20</v>
@@ -5926,7 +6135,7 @@
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="8" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>23</v>
@@ -5955,7 +6164,7 @@
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="8" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>21</v>
@@ -5983,7 +6192,7 @@
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>22</v>
@@ -6013,7 +6222,7 @@
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="8" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>90</v>
@@ -6042,7 +6251,7 @@
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="8" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>24</v>
@@ -6071,7 +6280,7 @@
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="8" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>25</v>
@@ -6129,7 +6338,7 @@
         <v>92</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="G15" s="23" t="str">
         <f t="shared" si="0"/>
@@ -6183,7 +6392,7 @@
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>26</v>
@@ -6240,7 +6449,7 @@
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>28</v>
@@ -6327,7 +6536,7 @@
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="8" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>41</v>
@@ -6359,7 +6568,7 @@
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>42</v>
@@ -6426,10 +6635,10 @@
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="8" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="G25" s="23" t="str">
         <f t="shared" si="0"/>
@@ -6516,7 +6725,7 @@
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="8" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="F28" s="8" t="s">
         <v>31</v>
@@ -6543,10 +6752,10 @@
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="8" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="G29" s="23" t="str">
         <f t="shared" si="0"/>
@@ -6576,7 +6785,7 @@
         <v>97</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="G30" s="23" t="str">
         <f t="shared" si="0"/>
@@ -6751,7 +6960,7 @@
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="8" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>48</v>
@@ -6783,7 +6992,7 @@
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="8" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="F37" s="8" t="s">
         <v>49</v>
@@ -6933,10 +7142,10 @@
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="G42" s="23" t="str">
         <f t="shared" si="1"/>
@@ -6963,7 +7172,7 @@
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="8" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="F43" s="8" t="s">
         <v>33</v>
@@ -6992,7 +7201,7 @@
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
       <c r="E44" s="8" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="F44" s="8" t="s">
         <v>33</v>
@@ -7022,7 +7231,7 @@
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
       <c r="E45" s="8" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="F45" s="8" t="s">
         <v>34</v>
@@ -7052,7 +7261,7 @@
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="8" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="F46" s="8" t="s">
         <v>53</v>
@@ -7083,7 +7292,7 @@
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="8" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="F47" s="8" t="s">
         <v>54</v>
@@ -7116,7 +7325,7 @@
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="8" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="F48" s="8" t="s">
         <v>55</v>
@@ -7145,7 +7354,7 @@
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
       <c r="E49" s="8" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="F49" s="8" t="s">
         <v>56</v>
@@ -7177,7 +7386,7 @@
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
       <c r="E50" s="8" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F50" s="8" t="s">
         <v>57</v>
@@ -7206,7 +7415,7 @@
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
       <c r="E51" s="8" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="F51" s="8" t="s">
         <v>35</v>
@@ -7239,10 +7448,10 @@
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
       <c r="E52" s="8" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="G52" s="23" t="str">
         <f t="shared" si="1"/>
@@ -7276,7 +7485,7 @@
         <v>60</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="F53" s="8" t="s">
         <v>36</v>
@@ -7313,7 +7522,7 @@
       </c>
       <c r="D54" s="7"/>
       <c r="E54" s="8" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="F54" s="8" t="s">
         <v>37</v>
@@ -7378,7 +7587,7 @@
       </c>
       <c r="D56" s="7"/>
       <c r="E56" s="8" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="F56" s="8" t="s">
         <v>38</v>
@@ -7409,7 +7618,7 @@
       </c>
       <c r="D57" s="7"/>
       <c r="E57" s="8" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="F57" s="8" t="s">
         <v>58</v>
@@ -7438,7 +7647,7 @@
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
       <c r="E58" s="8" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="F58" s="8" t="s">
         <v>39</v>
@@ -7467,10 +7676,10 @@
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
       <c r="E59" s="8" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="G59" s="23" t="str">
         <f t="shared" si="1"/>
@@ -7497,10 +7706,10 @@
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
       <c r="E60" s="8" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="G60" s="23" t="str">
         <f t="shared" si="1"/>
@@ -7526,10 +7735,10 @@
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
       <c r="E61" s="8" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="G61" s="23" t="str">
         <f t="shared" si="1"/>
@@ -7582,7 +7791,7 @@
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
       <c r="E63" s="8" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="F63" s="8" t="s">
         <v>59</v>
@@ -7610,7 +7819,7 @@
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
       <c r="E64" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F64" s="8" t="s">
         <v>60</v>
@@ -7639,7 +7848,7 @@
       <c r="C65" s="7"/>
       <c r="D65" s="7"/>
       <c r="E65" s="8" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="F65" s="8" t="s">
         <v>61</v>
@@ -7665,7 +7874,7 @@
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
       <c r="E66" s="8" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="F66" s="8" t="s">
         <v>60</v>
@@ -7693,7 +7902,7 @@
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
       <c r="E67" s="8" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="F67" s="8" t="s">
         <v>62</v>
@@ -7723,10 +7932,10 @@
       </c>
       <c r="D68" s="7"/>
       <c r="E68" s="8" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="F68" s="8" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="G68" s="23" t="str">
         <f t="shared" si="2"/>
@@ -7755,7 +7964,7 @@
       </c>
       <c r="D69" s="7"/>
       <c r="E69" s="8" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="F69" s="8" t="s">
         <v>63</v>
@@ -7785,7 +7994,7 @@
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
       <c r="E70" s="8" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="F70" s="8" t="s">
         <v>64</v>
@@ -7814,10 +8023,10 @@
       <c r="C71" s="7"/>
       <c r="D71" s="7"/>
       <c r="E71" s="8" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="F71" s="8" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="G71" s="23" t="str">
         <f t="shared" si="2"/>
@@ -7842,7 +8051,7 @@
       <c r="C72" s="7"/>
       <c r="D72" s="7"/>
       <c r="E72" s="8" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="F72" s="8" t="s">
         <v>65</v>
@@ -7874,7 +8083,7 @@
       </c>
       <c r="D73" s="7"/>
       <c r="E73" s="8" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="F73" s="8" t="s">
         <v>66</v>
@@ -7903,10 +8112,10 @@
       <c r="C74" s="12"/>
       <c r="D74" s="12"/>
       <c r="E74" s="13" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="F74" s="13" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="G74" s="24" t="str">
         <f t="shared" si="2"/>
@@ -7961,7 +8170,7 @@
   <sheetPr codeName="Feuil3"/>
   <dimension ref="A1:G108"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="45" zoomScaleNormal="45" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -7983,7 +8192,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>9</v>
@@ -7995,7 +8204,7 @@
         <v>11</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="400.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8008,7 +8217,7 @@
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="8" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>89</v>
@@ -8036,10 +8245,10 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="8" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G3" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8070,7 +8279,7 @@
         <v>70</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="G4" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8094,10 +8303,10 @@
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="8" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="G5" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8127,7 +8336,7 @@
         <v>162</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="G6" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8152,10 +8361,10 @@
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="8" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="G7" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8180,10 +8389,10 @@
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="8" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="G8" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8208,10 +8417,10 @@
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="8" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="G9" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8238,10 +8447,10 @@
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="8" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="G10" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8270,10 +8479,10 @@
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="8" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="G11" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8301,10 +8510,10 @@
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="8" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G12" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8331,7 +8540,7 @@
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="8" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>105</v>
@@ -8359,10 +8568,10 @@
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="8" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="G14" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8388,10 +8597,10 @@
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="8" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="G15" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8419,10 +8628,10 @@
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="8" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="G16" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8449,10 +8658,10 @@
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="8" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="G17" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8479,10 +8688,10 @@
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="8" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="G18" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8509,10 +8718,10 @@
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="8" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="G19" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8539,10 +8748,10 @@
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="8" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="G20" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8571,10 +8780,10 @@
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="8" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="G21" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8603,7 +8812,7 @@
         <v>163</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="G22" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8631,7 +8840,7 @@
         <v>164</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="G23" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8654,10 +8863,10 @@
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="8" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="G24" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8681,10 +8890,10 @@
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="8" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="G25" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8708,10 +8917,10 @@
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="8" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="G26" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8737,10 +8946,10 @@
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="8" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="G27" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8765,10 +8974,10 @@
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="8" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="G28" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8795,10 +9004,10 @@
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="8" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G29" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8824,10 +9033,10 @@
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="8" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G30" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8852,10 +9061,10 @@
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="8" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G31" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8880,10 +9089,10 @@
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="8" t="s">
-        <v>391</v>
+        <v>635</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="G32" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8893,7 +9102,7 @@
 I'm not here to appreciate the beauty of handmade art.[Wait=500][Space=2]
 I'm here to GET OFF THIS ISLAND![Wait=500] FUCK YOU, ART![Wait=500][Space=2]
 [Color=Gray]*CRACK*[Color=White]...[Wait=500][Space=2]
-Shit, I didn't know kicking a statue could dislocate its leg-.[Wait=500][Space=2]
+Shit, I didn't know kicking a statue could dislocate its leg-...[Wait=500][Space=2]
 [Color=Gray]*RUMBLE*[Color=White]...[Wait=500][Space=2]
 Huh?[Wait=500][Space=2]
 ]
@@ -8911,7 +9120,7 @@
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="8" t="s">
-        <v>393</v>
+        <v>636</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>106</v>
@@ -8921,7 +9130,7 @@
         <v>[Scene=32
 [Content=
 I-I don't know. The ground shook for a second...[Wait=500][Space=2]
-Wait...[Wait=500] What's tha-.[Wait=500][Space=2]
+Wait...[Wait=500] What's tha-...[Wait=500][Space=2]
 ...Did a motherfucking door just appear at the back of the museum?![Wait=500][Space=2]
 Did I really activate a mechanism at random because of my rage?[Wait=500][Space=2]
 ]
@@ -8940,7 +9149,7 @@
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="8" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>107</v>
@@ -8971,7 +9180,7 @@
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="8" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>108</v>
@@ -9003,10 +9212,10 @@
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="8" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="G36" s="23" t="str">
         <f t="shared" si="1"/>
@@ -9035,7 +9244,7 @@
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="8" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="F37" s="8" t="s">
         <v>109</v>
@@ -9063,7 +9272,7 @@
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="8" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>110</v>
@@ -9090,7 +9299,7 @@
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="E39" s="8" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>111</v>
@@ -9117,7 +9326,7 @@
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
       <c r="E40" s="8" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="F40" s="8" t="s">
         <v>112</v>
@@ -9144,7 +9353,7 @@
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
       <c r="E41" s="8" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="F41" s="8" t="s">
         <v>112</v>
@@ -9201,7 +9410,7 @@
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="8" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F43" s="8" t="s">
         <v>113</v>
@@ -9284,7 +9493,7 @@
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="8" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="F46" s="8" t="s">
         <v>114</v>
@@ -9341,7 +9550,7 @@
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="8" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="F48" s="8" t="s">
         <v>116</v>
@@ -9373,7 +9582,7 @@
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
       <c r="E49" s="8" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="F49" s="8" t="s">
         <v>117</v>
@@ -9407,7 +9616,7 @@
       </c>
       <c r="D50" s="7"/>
       <c r="E50" s="8" t="s">
-        <v>218</v>
+        <v>637</v>
       </c>
       <c r="F50" s="8" t="s">
         <v>118</v>
@@ -9417,7 +9626,7 @@
         <v>[Scene=49
 [Connection=2]
 [Content=
-[Color=Gray]*B[Beep=True]UZZ*[Color=White]...[Wait=500] That wasn't a reassuring sou-.[Wait=500][Space=2]
+[Color=Gray]*B[Beep=True]UZZ*[Color=White]...[Wait=500] That wasn't a reassuring sou-...[Wait=500][Space=2]
 [Color=Red]PASSWORD INCORRECT.[Wait=500] ENGAGING ANTI-INTRUDER PROTOCOL.[Color=White][Wait=500][Space=2]
 ...W-[Wait=500] What?[Wait=500] What does that even mean?[Wait=500][Space=2]
 [Color=Gray]*Cough*[Color=White]...[Wait=500] You gave me the wrong letter![Wait=500][Space=2]
@@ -9439,7 +9648,7 @@
       </c>
       <c r="D51" s="7"/>
       <c r="E51" s="8" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F51" s="8" t="s">
         <v>119</v>
@@ -9474,7 +9683,7 @@
         <v>166</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="G52" s="23" t="str">
         <f t="shared" si="1"/>
@@ -9503,7 +9712,7 @@
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
       <c r="E53" s="8" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F53" s="8" t="s">
         <v>121</v>
@@ -9564,7 +9773,7 @@
         <v>169</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G55" s="23" t="str">
         <f t="shared" si="1"/>
@@ -9643,7 +9852,7 @@
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
       <c r="E58" s="8" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="F58" s="8" t="s">
         <v>125</v>
@@ -9672,7 +9881,7 @@
         <v>172</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G59" s="23" t="str">
         <f t="shared" si="1"/>
@@ -9700,7 +9909,7 @@
         <v>72</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G60" s="23" t="str">
         <f t="shared" si="1"/>
@@ -9724,10 +9933,10 @@
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
       <c r="E61" s="8" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G61" s="23" t="str">
         <f t="shared" si="1"/>
@@ -9755,7 +9964,7 @@
         <v>73</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G62" s="23" t="str">
         <f t="shared" si="1"/>
@@ -9834,7 +10043,7 @@
       </c>
       <c r="D65" s="7"/>
       <c r="E65" s="8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F65" s="8" t="s">
         <v>128</v>
@@ -9863,10 +10072,10 @@
       </c>
       <c r="D66" s="7"/>
       <c r="E66" s="8" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F66" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G66" s="23" t="str">
         <f t="shared" ref="G66:G97" si="2">"[Scene=" &amp; A66 &amp; IF(OR(B66&lt;&gt;"",C66&lt;&gt;"",D66&lt;&gt;""),CHAR(10),"") &amp; IF(B66&lt;&gt;"","[BeepBack=" &amp; B66 &amp; "]","") &amp; IF(C66&lt;&gt;"","[Connection=" &amp; C66 &amp; "]","") &amp; IF(D66&lt;&gt;"","[Timer=" &amp; D66 &amp; "]","") &amp; IF(E66&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E66 &amp; CHAR(10) &amp; "]","") &amp; IF(F66&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F66 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
@@ -9891,7 +10100,7 @@
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
       <c r="E67" s="8" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="F67" s="8" t="s">
         <v>129</v>
@@ -9918,7 +10127,7 @@
       <c r="C68" s="7"/>
       <c r="D68" s="7"/>
       <c r="E68" s="8" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="F68" s="8" t="s">
         <v>130</v>
@@ -9945,7 +10154,7 @@
       <c r="C69" s="7"/>
       <c r="D69" s="7"/>
       <c r="E69" s="8" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="F69" s="8" t="s">
         <v>131</v>
@@ -10031,7 +10240,7 @@
         <v>7</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="F72" s="8" t="s">
         <v>134</v>
@@ -10061,7 +10270,7 @@
         <v>7</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="F73" s="8" t="s">
         <v>135</v>
@@ -10089,7 +10298,7 @@
       <c r="C74" s="7"/>
       <c r="D74" s="7"/>
       <c r="E74" s="8" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F74" s="8" t="s">
         <v>136</v>
@@ -10173,7 +10382,7 @@
       <c r="C77" s="7"/>
       <c r="D77" s="7"/>
       <c r="E77" s="8" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F77" s="8" t="s">
         <v>138</v>
@@ -10199,7 +10408,7 @@
       <c r="C78" s="7"/>
       <c r="D78" s="7"/>
       <c r="E78" s="8" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="F78" s="8" t="s">
         <v>138</v>
@@ -10253,7 +10462,7 @@
       <c r="C80" s="7"/>
       <c r="D80" s="7"/>
       <c r="E80" s="8" t="s">
-        <v>225</v>
+        <v>638</v>
       </c>
       <c r="F80" s="8" t="s">
         <v>140</v>
@@ -10264,7 +10473,7 @@
 [Content=
 [Color=Gray]*Footsteps*[Color=White]...[Wait=500] It's getting closer![Wait=500][Space=2]
 [Color=Gray]*SLAM*[Color=White]...[Wait=500][Space=2]
-I locked myself inside a room...[Wait=500] I think I'm safe n-.[Wait=500][Space=2]
+I locked myself inside a room...[Wait=500] I think I'm safe n-...[Wait=500][Space=2]
 [Color=Yellow]It's useless to hide, you know?[Wait=500] I know where you are at all times.[Color=White][Wait=500][Space=2]
 ]
 [Choices=
@@ -10365,7 +10574,7 @@
       <c r="C84" s="7"/>
       <c r="D84" s="7"/>
       <c r="E84" s="8" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="F84" s="8" t="s">
         <v>144</v>
@@ -10419,7 +10628,7 @@
       <c r="C86" s="7"/>
       <c r="D86" s="7"/>
       <c r="E86" s="8" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="F86" s="8" t="s">
         <v>146</v>
@@ -10476,10 +10685,10 @@
       <c r="C88" s="7"/>
       <c r="D88" s="7"/>
       <c r="E88" s="8" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="F88" s="8" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="G88" s="23" t="str">
         <f t="shared" si="2"/>
@@ -10504,7 +10713,7 @@
       <c r="C89" s="7"/>
       <c r="D89" s="7"/>
       <c r="E89" s="8" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="F89" s="8" t="s">
         <v>148</v>
@@ -10532,7 +10741,7 @@
       <c r="C90" s="7"/>
       <c r="D90" s="7"/>
       <c r="E90" s="8" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="F90" s="8" t="s">
         <v>149</v>
@@ -10595,10 +10804,10 @@
       </c>
       <c r="D92" s="7"/>
       <c r="E92" s="8" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="F92" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G92" s="23" t="str">
         <f t="shared" si="2"/>
@@ -10631,7 +10840,7 @@
         <v>87</v>
       </c>
       <c r="F93" s="8" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="G93" s="23" t="str">
         <f t="shared" si="2"/>
@@ -10664,7 +10873,7 @@
       </c>
       <c r="D94" s="7"/>
       <c r="E94" s="8" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F94" s="8" t="s">
         <v>151</v>
@@ -10694,7 +10903,7 @@
       <c r="C95" s="7"/>
       <c r="D95" s="7"/>
       <c r="E95" s="8" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="F95" s="8" t="s">
         <v>152</v>
@@ -10721,7 +10930,7 @@
       <c r="C96" s="7"/>
       <c r="D96" s="7"/>
       <c r="E96" s="8" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="F96" s="8" t="s">
         <v>153</v>
@@ -10751,7 +10960,7 @@
       <c r="C97" s="7"/>
       <c r="D97" s="7"/>
       <c r="E97" s="8" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="F97" s="8" t="s">
         <v>154</v>
@@ -10780,7 +10989,7 @@
       <c r="C98" s="7"/>
       <c r="D98" s="7"/>
       <c r="E98" s="8" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="F98" s="8" t="s">
         <v>155</v>
@@ -10845,7 +11054,7 @@
         <v>86</v>
       </c>
       <c r="F100" s="8" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="G100" s="23" t="str">
         <f t="shared" si="3"/>
@@ -10876,7 +11085,7 @@
       </c>
       <c r="D101" s="7"/>
       <c r="E101" s="8" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="F101" s="8" t="s">
         <v>157</v>
@@ -11032,7 +11241,7 @@
         <v>184</v>
       </c>
       <c r="F106" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G106" s="23" t="str">
         <f t="shared" si="3"/>
@@ -11058,7 +11267,7 @@
       <c r="C107" s="7"/>
       <c r="D107" s="7"/>
       <c r="E107" s="8" t="s">
-        <v>185</v>
+        <v>639</v>
       </c>
       <c r="F107" s="8" t="s">
         <v>161</v>
@@ -11067,7 +11276,7 @@
         <f t="shared" si="3"/>
         <v>[Scene=106
 [Content=
-Ahahah![Wait=500] That's tru-.[Wait=500][Space=2]
+Ahahah![Wait=500] That's tru-...[Wait=500][Space=2]
 [Color=Yellow]We have to go.[Color=White][Wait=500][Space=2]
 O-Oh...[Wait=500] Well, I guess it's a goodbye.[Wait=500][Space=2]
 I really hope to see you again.[Wait=500] Until then, believe in yourself.[Wait=500] I know we're great people.[Wait=500][Space=2]
@@ -11088,10 +11297,10 @@
       </c>
       <c r="D108" s="12"/>
       <c r="E108" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F108" s="13" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="G108" s="24" t="str">
         <f t="shared" si="3"/>
@@ -11153,7 +11362,7 @@
   <sheetPr codeName="Feuil4"/>
   <dimension ref="A1:G135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="45" zoomScaleNormal="45" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -11175,7 +11384,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>9</v>
@@ -11187,7 +11396,7 @@
         <v>11</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="400.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11200,10 +11409,10 @@
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="8" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G2" s="23" t="str">
         <f t="shared" ref="G2:G33" si="0">"[Scene=" &amp; A2 &amp; IF(OR(B2&lt;&gt;"",C2&lt;&gt;"",D2&lt;&gt;""),CHAR(10),"") &amp; IF(B2&lt;&gt;"","[BeepBack=" &amp; B2 &amp; "]","") &amp; IF(C2&lt;&gt;"","[Connection=" &amp; C2 &amp; "]","") &amp; IF(D2&lt;&gt;"","[Timer=" &amp; D2 &amp; "]","") &amp; IF(E2&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E2 &amp; CHAR(10) &amp; "]","") &amp; IF(F2&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F2 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
@@ -11228,10 +11437,10 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="8" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="G3" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11258,10 +11467,10 @@
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="8" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="G4" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11284,10 +11493,10 @@
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="8" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="G5" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11315,10 +11524,10 @@
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="8" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="G6" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11344,10 +11553,10 @@
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="8" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="G7" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11374,10 +11583,10 @@
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="8" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="G8" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11404,10 +11613,10 @@
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="8" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="G9" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11433,10 +11642,10 @@
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="8" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="G10" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11466,10 +11675,10 @@
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="8" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="G11" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11493,10 +11702,10 @@
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="8" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="G12" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11521,10 +11730,10 @@
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="8" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="G13" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11548,10 +11757,10 @@
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="8" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="G14" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11575,10 +11784,10 @@
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="8" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="G15" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11601,10 +11810,10 @@
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="8" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="G16" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11631,10 +11840,10 @@
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="8" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="G17" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11661,10 +11870,10 @@
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="8" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="G18" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11691,10 +11900,10 @@
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="8" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="G19" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11717,10 +11926,10 @@
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="8" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="G20" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11746,10 +11955,10 @@
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="8" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="G21" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11772,10 +11981,10 @@
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="8" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="G22" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11802,10 +12011,10 @@
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="8" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="G23" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11833,10 +12042,10 @@
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="8" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="G24" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11865,10 +12074,10 @@
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="8" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="G25" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11894,10 +12103,10 @@
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="8" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="G26" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11924,10 +12133,10 @@
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="8" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="G27" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11955,10 +12164,10 @@
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="8" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="G28" s="23" t="str">
         <f t="shared" si="0"/>
@@ -11983,10 +12192,10 @@
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="8" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="G29" s="23" t="str">
         <f t="shared" si="0"/>
@@ -12012,10 +12221,10 @@
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="8" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="G30" s="23" t="str">
         <f t="shared" si="0"/>
@@ -12041,10 +12250,10 @@
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="8" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="G31" s="23" t="str">
         <f t="shared" si="0"/>
@@ -12070,10 +12279,10 @@
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="8" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="G32" s="23" t="str">
         <f t="shared" si="0"/>
@@ -12098,10 +12307,10 @@
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="8" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="G33" s="23" t="str">
         <f t="shared" si="0"/>
@@ -12127,10 +12336,10 @@
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="8" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="G34" s="23" t="str">
         <f t="shared" ref="G34:G65" si="1">"[Scene=" &amp; A34 &amp; IF(OR(B34&lt;&gt;"",C34&lt;&gt;"",D34&lt;&gt;""),CHAR(10),"") &amp; IF(B34&lt;&gt;"","[BeepBack=" &amp; B34 &amp; "]","") &amp; IF(C34&lt;&gt;"","[Connection=" &amp; C34 &amp; "]","") &amp; IF(D34&lt;&gt;"","[Timer=" &amp; D34 &amp; "]","") &amp; IF(E34&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E34 &amp; CHAR(10) &amp; "]","") &amp; IF(F34&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F34 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
@@ -12155,10 +12364,10 @@
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="8" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="G35" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12182,10 +12391,10 @@
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="8" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="G36" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12211,10 +12420,10 @@
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="8" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="G37" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12239,10 +12448,10 @@
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="8" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="G38" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12270,10 +12479,10 @@
         <v>60</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="G39" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12303,10 +12512,10 @@
       </c>
       <c r="D40" s="7"/>
       <c r="E40" s="8" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="G40" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12336,10 +12545,10 @@
       </c>
       <c r="D41" s="7"/>
       <c r="E41" s="8" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="G41" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12373,10 +12582,10 @@
       </c>
       <c r="D42" s="7"/>
       <c r="E42" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="G42" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12404,10 +12613,10 @@
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="8" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G43" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12433,10 +12642,10 @@
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
       <c r="E44" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="G44" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12461,10 +12670,10 @@
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
       <c r="E45" s="8" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="G45" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12492,10 +12701,10 @@
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="8" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="G46" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12520,10 +12729,10 @@
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="8" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="G47" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12549,10 +12758,10 @@
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="8" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="G48" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12576,10 +12785,10 @@
       </c>
       <c r="D49" s="7"/>
       <c r="E49" s="8" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="G49" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12612,10 +12821,10 @@
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
       <c r="E50" s="8" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G50" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12641,10 +12850,10 @@
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
       <c r="E51" s="8" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="G51" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12667,10 +12876,10 @@
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
       <c r="E52" s="8" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="G52" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12696,10 +12905,10 @@
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
       <c r="E53" s="8" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="G53" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12726,10 +12935,10 @@
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
       <c r="E54" s="8" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="G54" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12753,10 +12962,10 @@
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
       <c r="E55" s="8" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="G55" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12780,10 +12989,10 @@
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
       <c r="E56" s="8" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="G56" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12807,10 +13016,10 @@
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
       <c r="E57" s="8" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="G57" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12834,10 +13043,10 @@
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
       <c r="E58" s="8" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="G58" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12861,10 +13070,10 @@
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
       <c r="E59" s="8" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="G59" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12892,10 +13101,10 @@
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
       <c r="E60" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="G60" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12921,10 +13130,10 @@
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
       <c r="E61" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="G61" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12949,10 +13158,10 @@
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
       <c r="E62" s="8" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="G62" s="23" t="str">
         <f t="shared" si="1"/>
@@ -12979,10 +13188,10 @@
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
       <c r="E63" s="8" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="G63" s="23" t="str">
         <f t="shared" si="1"/>
@@ -13008,10 +13217,10 @@
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
       <c r="E64" s="8" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="G64" s="23" t="str">
         <f t="shared" si="1"/>
@@ -13036,10 +13245,10 @@
       <c r="C65" s="7"/>
       <c r="D65" s="7"/>
       <c r="E65" s="8" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="F65" s="8" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G65" s="23" t="str">
         <f t="shared" si="1"/>
@@ -13069,10 +13278,10 @@
         <v>5</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>522</v>
+        <v>633</v>
       </c>
       <c r="F66" s="8" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="G66" s="23" t="str">
         <f t="shared" ref="G66:G74" si="2">"[Scene=" &amp; A66 &amp; IF(OR(B66&lt;&gt;"",C66&lt;&gt;"",D66&lt;&gt;""),CHAR(10),"") &amp; IF(B66&lt;&gt;"","[BeepBack=" &amp; B66 &amp; "]","") &amp; IF(C66&lt;&gt;"","[Connection=" &amp; C66 &amp; "]","") &amp; IF(D66&lt;&gt;"","[Timer=" &amp; D66 &amp; "]","") &amp; IF(E66&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E66 &amp; CHAR(10) &amp; "]","") &amp; IF(F66&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F66 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
@@ -13080,7 +13289,7 @@
 [Connection=2][Timer=5]
 [Content=
 Left it is![Wait=500][Space=2]
-Well tha-.[Wait=500][Space=2]
+Well tha-...[Wait=500][Space=2]
 Fuck.[Wait=500] I heard something behind me.[Wait=500][Space=2]
 Oh no...[Wait=500] OH SHIT SHIT SHIT IT'S RUNNING TOWARDS ME!!![Wait=500][Space=2]
 WHERE DO I GO?! QUICK!!![Wait=500][Space=2]
@@ -13103,10 +13312,10 @@
       </c>
       <c r="D67" s="7"/>
       <c r="E67" s="8" t="s">
-        <v>523</v>
+        <v>634</v>
       </c>
       <c r="F67" s="8" t="s">
-        <v>524</v>
+        <v>517</v>
       </c>
       <c r="G67" s="23" t="str">
         <f t="shared" si="2"/>
@@ -13115,7 +13324,7 @@
 [Content=
 Are you sure it's this way?![Wait=500][Space=2]
 There's something strange about this pla-[Color=Gray]*Cracking noises*[Color=White]...[Wait=500][Space=2]
-...[Wait=500] Don't tell me the ground is-.[Wait=500][Space=2]
+...[Wait=500] Don't tell me the ground is-...[Wait=500][Space=2]
 [Color=Gray]*COLLAPSING RUCKUS*[Color=White]...[Wait=500][Space=2]
 WOAAAAAAH SHIIII-[Color=Gray]*THUD*[Color=White]...[Wait=500][Space=2]
 ]
@@ -13135,10 +13344,10 @@
       </c>
       <c r="D68" s="7"/>
       <c r="E68" s="8" t="s">
-        <v>525</v>
+        <v>518</v>
       </c>
       <c r="F68" s="8" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="G68" s="23" t="str">
         <f t="shared" si="2"/>
@@ -13166,10 +13375,10 @@
       </c>
       <c r="D69" s="7"/>
       <c r="E69" s="8" t="s">
-        <v>526</v>
+        <v>519</v>
       </c>
       <c r="F69" s="8" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
       <c r="G69" s="23" t="str">
         <f t="shared" si="2"/>
@@ -13197,10 +13406,10 @@
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
       <c r="E70" s="8" t="s">
-        <v>528</v>
+        <v>521</v>
       </c>
       <c r="F70" s="8" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G70" s="23" t="str">
         <f t="shared" si="2"/>
@@ -13225,10 +13434,10 @@
       <c r="C71" s="7"/>
       <c r="D71" s="7"/>
       <c r="E71" s="8" t="s">
-        <v>529</v>
+        <v>522</v>
       </c>
       <c r="F71" s="8" t="s">
-        <v>530</v>
+        <v>523</v>
       </c>
       <c r="G71" s="23" t="str">
         <f t="shared" si="2"/>
@@ -13254,10 +13463,10 @@
       <c r="C72" s="7"/>
       <c r="D72" s="7"/>
       <c r="E72" s="8" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="F72" s="8" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G72" s="23" t="str">
         <f t="shared" si="2"/>
@@ -13286,10 +13495,10 @@
       <c r="C73" s="7"/>
       <c r="D73" s="7"/>
       <c r="E73" s="8" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="F73" s="8" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="G73" s="23" t="str">
         <f t="shared" si="2"/>
@@ -13315,10 +13524,10 @@
       <c r="C74" s="12"/>
       <c r="D74" s="12"/>
       <c r="E74" s="13" t="s">
-        <v>534</v>
+        <v>527</v>
       </c>
       <c r="F74" s="13" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
       <c r="G74" s="24" t="str">
         <f t="shared" si="2"/>
@@ -13344,10 +13553,10 @@
       <c r="C75" s="7"/>
       <c r="D75" s="7"/>
       <c r="E75" s="8" t="s">
-        <v>536</v>
+        <v>529</v>
       </c>
       <c r="F75" s="8" t="s">
-        <v>537</v>
+        <v>530</v>
       </c>
       <c r="G75" s="23" t="str">
         <f>"[Scene=" &amp; A75 &amp; IF(OR(B75&lt;&gt;"",C75&lt;&gt;"",D75&lt;&gt;""),CHAR(10),"") &amp; IF(B75&lt;&gt;"","[BeepBack=" &amp; B75 &amp; "]","") &amp; IF(C75&lt;&gt;"","[Connection=" &amp; C75 &amp; "]","") &amp; IF(D75&lt;&gt;"","[Timer=" &amp; D75 &amp; "]","") &amp; IF(E75&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E75 &amp; CHAR(10) &amp; "]","") &amp; IF(F75&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F75 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
@@ -13371,10 +13580,10 @@
       <c r="C76" s="7"/>
       <c r="D76" s="7"/>
       <c r="E76" s="8" t="s">
-        <v>538</v>
+        <v>531</v>
       </c>
       <c r="F76" s="8" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
       <c r="G76" s="23" t="str">
         <f>"[Scene=" &amp; A76 &amp; IF(OR(B76&lt;&gt;"",C76&lt;&gt;"",D76&lt;&gt;""),CHAR(10),"") &amp; IF(B76&lt;&gt;"","[BeepBack=" &amp; B76 &amp; "]","") &amp; IF(C76&lt;&gt;"","[Connection=" &amp; C76 &amp; "]","") &amp; IF(D76&lt;&gt;"","[Timer=" &amp; D76 &amp; "]","") &amp; IF(E76&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E76 &amp; CHAR(10) &amp; "]","") &amp; IF(F76&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F76 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
@@ -13399,10 +13608,10 @@
       <c r="C77" s="7"/>
       <c r="D77" s="7"/>
       <c r="E77" s="8" t="s">
-        <v>540</v>
+        <v>533</v>
       </c>
       <c r="F77" s="8" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
       <c r="G77" s="23" t="str">
         <f t="shared" ref="G77:G83" si="3">"[Scene=" &amp; A77 &amp; IF(OR(B77&lt;&gt;"",C77&lt;&gt;"",D77&lt;&gt;""),CHAR(10),"") &amp; IF(B77&lt;&gt;"","[BeepBack=" &amp; B77 &amp; "]","") &amp; IF(C77&lt;&gt;"","[Connection=" &amp; C77 &amp; "]","") &amp; IF(D77&lt;&gt;"","[Timer=" &amp; D77 &amp; "]","") &amp; IF(E77&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E77 &amp; CHAR(10) &amp; "]","") &amp; IF(F77&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F77 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
@@ -13428,10 +13637,10 @@
       <c r="C78" s="7"/>
       <c r="D78" s="7"/>
       <c r="E78" s="8" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
       <c r="F78" s="8" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
       <c r="G78" s="23" t="str">
         <f t="shared" si="3"/>
@@ -13458,10 +13667,10 @@
       <c r="C79" s="7"/>
       <c r="D79" s="7"/>
       <c r="E79" s="8" t="s">
-        <v>544</v>
+        <v>537</v>
       </c>
       <c r="F79" s="8" t="s">
-        <v>545</v>
+        <v>538</v>
       </c>
       <c r="G79" s="23" t="str">
         <f t="shared" si="3"/>
@@ -13490,10 +13699,10 @@
       <c r="C80" s="7"/>
       <c r="D80" s="7"/>
       <c r="E80" s="8" t="s">
-        <v>546</v>
+        <v>539</v>
       </c>
       <c r="F80" s="8" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
       <c r="G80" s="23" t="str">
         <f t="shared" si="3"/>
@@ -13521,10 +13730,10 @@
       <c r="C81" s="7"/>
       <c r="D81" s="7"/>
       <c r="E81" s="8" t="s">
-        <v>548</v>
+        <v>541</v>
       </c>
       <c r="F81" s="8" t="s">
-        <v>549</v>
+        <v>542</v>
       </c>
       <c r="G81" s="23" t="str">
         <f t="shared" si="3"/>
@@ -13554,10 +13763,10 @@
       </c>
       <c r="D82" s="7"/>
       <c r="E82" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F82" s="8" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="G82" s="23" t="str">
         <f t="shared" si="3"/>
@@ -13587,10 +13796,10 @@
       </c>
       <c r="D83" s="12"/>
       <c r="E83" s="13" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F83" s="13" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="G83" s="24" t="str">
         <f t="shared" si="3"/>
@@ -13620,10 +13829,10 @@
       </c>
       <c r="D84" s="7"/>
       <c r="E84" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F84" s="8" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="G84" s="23" t="str">
         <f t="shared" ref="G84:G92" si="4">"[Scene=" &amp; A84 &amp; IF(OR(B84&lt;&gt;"",C84&lt;&gt;"",D84&lt;&gt;""),CHAR(10),"") &amp; IF(B84&lt;&gt;"","[BeepBack=" &amp; B84 &amp; "]","") &amp; IF(C84&lt;&gt;"","[Connection=" &amp; C84 &amp; "]","") &amp; IF(D84&lt;&gt;"","[Timer=" &amp; D84 &amp; "]","") &amp; IF(E84&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E84 &amp; CHAR(10) &amp; "]","") &amp; IF(F84&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F84 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
@@ -13652,10 +13861,10 @@
       <c r="C85" s="7"/>
       <c r="D85" s="7"/>
       <c r="E85" s="8" t="s">
-        <v>550</v>
+        <v>543</v>
       </c>
       <c r="F85" s="8" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G85" s="23" t="str">
         <f t="shared" si="4"/>
@@ -13679,10 +13888,10 @@
       <c r="C86" s="7"/>
       <c r="D86" s="7"/>
       <c r="E86" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F86" s="8" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="G86" s="23" t="str">
         <f t="shared" si="4"/>
@@ -13708,10 +13917,10 @@
       <c r="C87" s="7"/>
       <c r="D87" s="7"/>
       <c r="E87" s="8" t="s">
-        <v>551</v>
+        <v>544</v>
       </c>
       <c r="F87" s="8" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="G87" s="23" t="str">
         <f t="shared" si="4"/>
@@ -13736,10 +13945,10 @@
       <c r="C88" s="7"/>
       <c r="D88" s="7"/>
       <c r="E88" s="8" t="s">
-        <v>552</v>
+        <v>545</v>
       </c>
       <c r="F88" s="8" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
       <c r="G88" s="23" t="str">
         <f t="shared" si="4"/>
@@ -13766,10 +13975,10 @@
       <c r="C89" s="7"/>
       <c r="D89" s="7"/>
       <c r="E89" s="8" t="s">
-        <v>554</v>
+        <v>547</v>
       </c>
       <c r="F89" s="8" t="s">
-        <v>555</v>
+        <v>548</v>
       </c>
       <c r="G89" s="23" t="str">
         <f t="shared" si="4"/>
@@ -13794,10 +14003,10 @@
       <c r="C90" s="7"/>
       <c r="D90" s="7"/>
       <c r="E90" s="8" t="s">
-        <v>556</v>
+        <v>549</v>
       </c>
       <c r="F90" s="8" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
       <c r="G90" s="23" t="str">
         <f t="shared" si="4"/>
@@ -13822,10 +14031,10 @@
       <c r="C91" s="7"/>
       <c r="D91" s="7"/>
       <c r="E91" s="8" t="s">
-        <v>558</v>
+        <v>551</v>
       </c>
       <c r="F91" s="8" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
       <c r="G91" s="23" t="str">
         <f t="shared" si="4"/>
@@ -13852,10 +14061,10 @@
       <c r="C92" s="12"/>
       <c r="D92" s="12"/>
       <c r="E92" s="13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F92" s="13" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="G92" s="24" t="str">
         <f t="shared" si="4"/>
@@ -13885,10 +14094,10 @@
         <v>10</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="F93" s="8" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G93" s="23" t="str">
         <f t="shared" ref="G93:G135" si="5">"[Scene=" &amp; A93 &amp; IF(OR(B93&lt;&gt;"",C93&lt;&gt;"",D93&lt;&gt;""),CHAR(10),"") &amp; IF(B93&lt;&gt;"","[BeepBack=" &amp; B93 &amp; "]","") &amp; IF(C93&lt;&gt;"","[Connection=" &amp; C93 &amp; "]","") &amp; IF(D93&lt;&gt;"","[Timer=" &amp; D93 &amp; "]","") &amp; IF(E93&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E93 &amp; CHAR(10) &amp; "]","") &amp; IF(F93&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F93 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
@@ -13919,10 +14128,10 @@
         <v>10</v>
       </c>
       <c r="E94" s="8" t="s">
-        <v>561</v>
+        <v>554</v>
       </c>
       <c r="F94" s="8" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="G94" s="23" t="str">
         <f t="shared" si="5"/>
@@ -13952,10 +14161,10 @@
         <v>10</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>562</v>
+        <v>555</v>
       </c>
       <c r="F95" s="8" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="G95" s="23" t="str">
         <f t="shared" si="5"/>
@@ -13987,10 +14196,10 @@
       </c>
       <c r="D96" s="7"/>
       <c r="E96" s="8" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="F96" s="8" t="s">
-        <v>564</v>
+        <v>557</v>
       </c>
       <c r="G96" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14019,10 +14228,10 @@
       <c r="C97" s="7"/>
       <c r="D97" s="7"/>
       <c r="E97" s="8" t="s">
-        <v>565</v>
+        <v>558</v>
       </c>
       <c r="F97" s="8" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="G97" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14050,10 +14259,10 @@
       </c>
       <c r="D98" s="7"/>
       <c r="E98" s="8" t="s">
-        <v>566</v>
+        <v>559</v>
       </c>
       <c r="F98" s="8" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="G98" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14081,10 +14290,10 @@
       </c>
       <c r="D99" s="7"/>
       <c r="E99" s="8" t="s">
-        <v>567</v>
+        <v>560</v>
       </c>
       <c r="F99" s="8" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="G99" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14113,10 +14322,10 @@
       </c>
       <c r="D100" s="7"/>
       <c r="E100" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F100" s="8" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="G100" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14147,10 +14356,10 @@
       </c>
       <c r="D101" s="7"/>
       <c r="E101" s="8" t="s">
-        <v>568</v>
+        <v>561</v>
       </c>
       <c r="F101" s="8" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G101" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14180,10 +14389,10 @@
       </c>
       <c r="D102" s="7"/>
       <c r="E102" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F102" s="8" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="G102" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14211,10 +14420,10 @@
       </c>
       <c r="D103" s="7"/>
       <c r="E103" s="8" t="s">
-        <v>569</v>
+        <v>562</v>
       </c>
       <c r="F103" s="8" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="G103" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14243,10 +14452,10 @@
       <c r="C104" s="7"/>
       <c r="D104" s="7"/>
       <c r="E104" s="8" t="s">
-        <v>570</v>
+        <v>563</v>
       </c>
       <c r="F104" s="8" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G104" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14272,10 +14481,10 @@
       <c r="C105" s="7"/>
       <c r="D105" s="7"/>
       <c r="E105" s="8" t="s">
-        <v>571</v>
+        <v>564</v>
       </c>
       <c r="F105" s="8" t="s">
-        <v>572</v>
+        <v>565</v>
       </c>
       <c r="G105" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14302,10 +14511,10 @@
       <c r="C106" s="7"/>
       <c r="D106" s="7"/>
       <c r="E106" s="8" t="s">
-        <v>573</v>
+        <v>566</v>
       </c>
       <c r="F106" s="8" t="s">
-        <v>574</v>
+        <v>567</v>
       </c>
       <c r="G106" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14329,10 +14538,10 @@
       <c r="C107" s="7"/>
       <c r="D107" s="7"/>
       <c r="E107" s="8" t="s">
-        <v>575</v>
+        <v>568</v>
       </c>
       <c r="F107" s="8" t="s">
-        <v>576</v>
+        <v>569</v>
       </c>
       <c r="G107" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14357,10 +14566,10 @@
       <c r="C108" s="7"/>
       <c r="D108" s="7"/>
       <c r="E108" s="8" t="s">
-        <v>577</v>
+        <v>570</v>
       </c>
       <c r="F108" s="8" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G108" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14387,10 +14596,10 @@
       <c r="C109" s="7"/>
       <c r="D109" s="7"/>
       <c r="E109" s="8" t="s">
-        <v>578</v>
+        <v>571</v>
       </c>
       <c r="F109" s="8" t="s">
-        <v>574</v>
+        <v>567</v>
       </c>
       <c r="G109" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14416,10 +14625,10 @@
       <c r="C110" s="7"/>
       <c r="D110" s="7"/>
       <c r="E110" s="8" t="s">
-        <v>579</v>
+        <v>572</v>
       </c>
       <c r="F110" s="8" t="s">
-        <v>574</v>
+        <v>567</v>
       </c>
       <c r="G110" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14446,10 +14655,10 @@
       <c r="C111" s="7"/>
       <c r="D111" s="7"/>
       <c r="E111" s="8" t="s">
-        <v>580</v>
+        <v>573</v>
       </c>
       <c r="F111" s="8" t="s">
-        <v>574</v>
+        <v>567</v>
       </c>
       <c r="G111" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14474,10 +14683,10 @@
       <c r="C112" s="7"/>
       <c r="D112" s="7"/>
       <c r="E112" s="8" t="s">
-        <v>581</v>
+        <v>574</v>
       </c>
       <c r="F112" s="8" t="s">
-        <v>574</v>
+        <v>567</v>
       </c>
       <c r="G112" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14501,10 +14710,10 @@
       <c r="C113" s="7"/>
       <c r="D113" s="7"/>
       <c r="E113" s="8" t="s">
-        <v>582</v>
+        <v>575</v>
       </c>
       <c r="F113" s="8" t="s">
-        <v>583</v>
+        <v>576</v>
       </c>
       <c r="G113" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14531,10 +14740,10 @@
       <c r="C114" s="7"/>
       <c r="D114" s="7"/>
       <c r="E114" s="8" t="s">
-        <v>584</v>
+        <v>577</v>
       </c>
       <c r="F114" s="8" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="G114" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14561,10 +14770,10 @@
       <c r="C115" s="7"/>
       <c r="D115" s="7"/>
       <c r="E115" s="8" t="s">
-        <v>585</v>
+        <v>578</v>
       </c>
       <c r="F115" s="8" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="G115" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14589,10 +14798,10 @@
       <c r="C116" s="7"/>
       <c r="D116" s="7"/>
       <c r="E116" s="8" t="s">
-        <v>586</v>
+        <v>579</v>
       </c>
       <c r="F116" s="8" t="s">
-        <v>587</v>
+        <v>580</v>
       </c>
       <c r="G116" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14618,10 +14827,10 @@
       <c r="C117" s="7"/>
       <c r="D117" s="7"/>
       <c r="E117" s="8" t="s">
-        <v>588</v>
+        <v>581</v>
       </c>
       <c r="F117" s="8" t="s">
-        <v>589</v>
+        <v>582</v>
       </c>
       <c r="G117" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14645,10 +14854,10 @@
       <c r="C118" s="7"/>
       <c r="D118" s="7"/>
       <c r="E118" s="8" t="s">
-        <v>590</v>
+        <v>583</v>
       </c>
       <c r="F118" s="8" t="s">
-        <v>591</v>
+        <v>584</v>
       </c>
       <c r="G118" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14672,10 +14881,10 @@
       <c r="C119" s="7"/>
       <c r="D119" s="7"/>
       <c r="E119" s="8" t="s">
-        <v>592</v>
+        <v>585</v>
       </c>
       <c r="F119" s="8" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G119" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14704,10 +14913,10 @@
       <c r="C120" s="7"/>
       <c r="D120" s="7"/>
       <c r="E120" s="8" t="s">
-        <v>593</v>
+        <v>586</v>
       </c>
       <c r="F120" s="8" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="G120" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14732,10 +14941,10 @@
       <c r="C121" s="7"/>
       <c r="D121" s="7"/>
       <c r="E121" s="8" t="s">
-        <v>594</v>
+        <v>587</v>
       </c>
       <c r="F121" s="8" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="G121" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14763,10 +14972,10 @@
       <c r="C122" s="7"/>
       <c r="D122" s="7"/>
       <c r="E122" s="8" t="s">
-        <v>595</v>
+        <v>588</v>
       </c>
       <c r="F122" s="8" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="G122" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14791,10 +15000,10 @@
       <c r="C123" s="7"/>
       <c r="D123" s="7"/>
       <c r="E123" s="8" t="s">
-        <v>596</v>
+        <v>589</v>
       </c>
       <c r="F123" s="8" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G123" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14819,10 +15028,10 @@
       <c r="C124" s="7"/>
       <c r="D124" s="7"/>
       <c r="E124" s="8" t="s">
-        <v>597</v>
+        <v>590</v>
       </c>
       <c r="F124" s="8" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G124" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14848,10 +15057,10 @@
       <c r="C125" s="7"/>
       <c r="D125" s="7"/>
       <c r="E125" s="8" t="s">
-        <v>598</v>
+        <v>591</v>
       </c>
       <c r="F125" s="8" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="G125" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14879,10 +15088,10 @@
       <c r="C126" s="7"/>
       <c r="D126" s="7"/>
       <c r="E126" s="8" t="s">
-        <v>599</v>
+        <v>592</v>
       </c>
       <c r="F126" s="8" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="G126" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14907,10 +15116,10 @@
       <c r="C127" s="7"/>
       <c r="D127" s="7"/>
       <c r="E127" s="8" t="s">
-        <v>600</v>
+        <v>593</v>
       </c>
       <c r="F127" s="8" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="G127" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14936,10 +15145,10 @@
       <c r="C128" s="7"/>
       <c r="D128" s="7"/>
       <c r="E128" s="8" t="s">
-        <v>601</v>
+        <v>594</v>
       </c>
       <c r="F128" s="8" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="G128" s="23" t="str">
         <f t="shared" si="5"/>
@@ -14969,10 +15178,10 @@
       </c>
       <c r="D129" s="7"/>
       <c r="E129" s="8" t="s">
-        <v>602</v>
+        <v>595</v>
       </c>
       <c r="F129" s="8" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="G129" s="23" t="str">
         <f t="shared" si="5"/>
@@ -15001,10 +15210,10 @@
       </c>
       <c r="D130" s="7"/>
       <c r="E130" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F130" s="8" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="G130" s="23" t="str">
         <f t="shared" si="5"/>
@@ -15033,10 +15242,10 @@
       <c r="C131" s="7"/>
       <c r="D131" s="7"/>
       <c r="E131" s="8" t="s">
-        <v>603</v>
+        <v>596</v>
       </c>
       <c r="F131" s="8" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="G131" s="23" t="str">
         <f t="shared" si="5"/>
@@ -15061,10 +15270,10 @@
       <c r="C132" s="7"/>
       <c r="D132" s="7"/>
       <c r="E132" s="8" t="s">
-        <v>604</v>
+        <v>597</v>
       </c>
       <c r="F132" s="8" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="G132" s="23" t="str">
         <f t="shared" si="5"/>
@@ -15089,10 +15298,10 @@
       <c r="C133" s="7"/>
       <c r="D133" s="7"/>
       <c r="E133" s="8" t="s">
-        <v>605</v>
+        <v>598</v>
       </c>
       <c r="F133" s="8" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="G133" s="23" t="str">
         <f t="shared" si="5"/>
@@ -15122,10 +15331,10 @@
       </c>
       <c r="D134" s="7"/>
       <c r="E134" s="8" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="F134" s="8" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G134" s="23" t="str">
         <f t="shared" si="5"/>
@@ -15156,10 +15365,10 @@
       </c>
       <c r="D135" s="7"/>
       <c r="E135" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F135" s="8" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="G135" s="23" t="str">
         <f t="shared" si="5"/>
@@ -15221,8 +15430,8 @@
   <sheetPr codeName="Feuil5"/>
   <dimension ref="A1:G151"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C151" sqref="C151"/>
+    <sheetView tabSelected="1" topLeftCell="D31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.7109375" defaultRowHeight="400.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -15243,7 +15452,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>9</v>
@@ -15255,7 +15464,7 @@
         <v>11</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="400.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -15263,13 +15472,29 @@
         <v>1</v>
       </c>
       <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
+      <c r="C2" s="7">
+        <v>3</v>
+      </c>
       <c r="D2" s="7"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="E2" s="8" t="s">
+        <v>601</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>604</v>
+      </c>
       <c r="G2" s="23" t="str">
         <f t="shared" ref="G2:G33" si="0">"[Scene=" &amp; A2 &amp; IF(OR(B2&lt;&gt;"",C2&lt;&gt;"",D2&lt;&gt;""),CHAR(10),"") &amp; IF(B2&lt;&gt;"","[BeepBack=" &amp; B2 &amp; "]","") &amp; IF(C2&lt;&gt;"","[Connection=" &amp; C2 &amp; "]","") &amp; IF(D2&lt;&gt;"","[Timer=" &amp; D2 &amp; "]","") &amp; IF(E2&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E2 &amp; CHAR(10) &amp; "]","") &amp; IF(F2&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F2 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
         <v>[Scene=1
+[Connection=3]
+[Content=
+Yeah.[Wait=500] Of all places, the factory seems like the place I could find answers and the key to my escape.[Wait=500][Space=2]
+I'll go there if I can.[Wait=500] Let's go.[Wait=500][Space=2]
+[Color=Gray]*Footsteps*[Color=White]...[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=2][NextSceneNoTrust=3][TrustNeed=50][Content=What exactly do you mean by key?]]
+[Choice2=[NextScene=9][NextSceneNoTrust=10][TrustNeed=50][Content=If you can? Would there be anything preventing you?]]
+]
 ]</v>
       </c>
     </row>
@@ -15280,11 +15505,24 @@
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
+      <c r="E3" s="8" t="s">
+        <v>600</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>605</v>
+      </c>
       <c r="G3" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=2
+[Content=
+With how much all of this looks like a setup, I might find the fuse there.[Wait=500][Space=2]
+I just don't get why whoever is keeping me in this place left a working phone back in the supermarket.[Wait=500][Space=2]
+I'm just playing their game at this point.[Wait=500][Space=2]
+[Color=Gray]*Footsteps*[Color=White]...[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=8][Content=That's a pain of a situation for sure.]]
+]
 ]</v>
       </c>
     </row>
@@ -15295,11 +15533,23 @@
       <c r="B4" s="6"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
+      <c r="E4" s="8" t="s">
+        <v>602</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>606</v>
+      </c>
       <c r="G4" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=3
+[Content=
+...[Wait=500] I hope I can find the fuse, why are you asking?[Wait=500][Space=2]
+[Color=Gray]*Footsteps*[Color=White]...[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=4][Content=Are you... alright?]]
+[Choice2=[NextScene=7][Content=Of course. Just making sure.]]
+]
 ]</v>
       </c>
     </row>
@@ -15310,11 +15560,27 @@
       <c r="B5" s="6"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+      <c r="E5" s="8" t="s">
+        <v>640</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>607</v>
+      </c>
       <c r="G5" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=4
+[Content=
+I...[Wait=500] I'm just really stressed-...[Wait=500][Space=2]
+...[Wait=500][Space=2]
+Listen, I might have found this phone but I don't feel like you're here to help...[Wait=500][Space=2]
+I don't know, you've got to put yourself in my place a bit...[Wait=500][Space=2]
+[Color=Gray]*Footsteps*[Color=White]...[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=5][TrustAdd=25][Content=It's my fault, I behaved like an idiot.]]
+[Choice2=[NextScene=7][Content=You're right, let's both calm down and work together.]]
+[Choice3=[NextScene=7][Content=I'm sorry, I wasn't expecting a call like that.]]
+]
 ]</v>
       </c>
     </row>
@@ -15325,11 +15591,24 @@
       <c r="B6" s="6"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
+      <c r="E6" s="8" t="s">
+        <v>603</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>608</v>
+      </c>
       <c r="G6" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=5
+[Content=
+You- I mean, you know-...[Wait=500] I get it.[Wait=500][Space=2]
+It's hard to handle some random person calling you for seemingly no reason.[Wait=500][Space=2]
+...[Wait=500][Space=2]
+But thanks for admitting that, I already feel safer if you're able to show a bit of self-awareness.[Wait=500][Space=2]
+]
+[Choices=
+[Choice1=[NextScene=6][Content=We're cool then!]]
+]
 ]</v>
       </c>
     </row>
@@ -15340,11 +15619,21 @@
       <c r="B7" s="6"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
-      <c r="E7" s="8"/>
+      <c r="E7" s="8" t="s">
+        <v>609</v>
+      </c>
       <c r="F7" s="8"/>
       <c r="G7" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=6
+[Content=
+We are.[Wait=500][Space=2]
+...[Wait=500][Space=2]
+I've arrived to the entrance, but I have to get through a fence.[Wait=500][Space=2]
+It seems really fragile, so getting rid of it wouldn't be that hard.[Wait=500] That thing's already quite damaged.[Wait=500][Space=2]
+...[Wait=500][Space=2]
+Or I could go around, there's no reason for a building like this not to have some kind of backdoor.[Wait=500][Space=2]
+]
 ]</v>
       </c>
     </row>
@@ -15355,11 +15644,19 @@
       <c r="B8" s="6"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
-      <c r="E8" s="8"/>
+      <c r="E8" s="8" t="s">
+        <v>610</v>
+      </c>
       <c r="F8" s="8"/>
       <c r="G8" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=7
+[Content=
+Alright...[Wait=500][Space=2]
+...[Wait=500][Space=2]
+There's a metal fence around the entrance.[Wait=500][Space=2]
+I should be able to push it, but going around and finding another entrance might be easier.[Wait=500][Space=2]
+]
 ]</v>
       </c>
     </row>
@@ -15370,11 +15667,20 @@
       <c r="B9" s="6"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
-      <c r="E9" s="8"/>
+      <c r="E9" s="8" t="s">
+        <v>611</v>
+      </c>
       <c r="F9" s="8"/>
       <c r="G9" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=8
+[Content=
+Kind of...[Wait=500] Yeah.[Wait=500][Space=2]
+...[Wait=500][Space=2]
+I got closer to the building, enough to realise the entrance's blocked by a fence.[Wait=500][Space=2]
+It looks brittle enough, but getting around might also be easier.[Wait=500][Space=2]
+It only seems to block the main entrance.[Wait=500][Space=2]
+]
 ]</v>
       </c>
     </row>
@@ -15385,11 +15691,20 @@
       <c r="B10" s="6"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
-      <c r="E10" s="8"/>
+      <c r="E10" s="8" t="s">
+        <v>612</v>
+      </c>
       <c r="F10" s="8"/>
       <c r="G10" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=9
+[Content=
+There seem to be a fence in front of the main entrance.[Wait=500][Space=2]
+I probably could get around and find another way to enter.[Wait=500][Space=2]
+But from this distance it looks really thin and rusted.[Wait=500][Space=2]
+I think pushing it down and getting over would prove quite easy.[Wait=500][Space=2]
+What do you think?[Wait=500][Space=2]
+]
 ]</v>
       </c>
     </row>
@@ -15400,11 +15715,16 @@
       <c r="B11" s="6"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
-      <c r="E11" s="8"/>
+      <c r="E11" s="8" t="s">
+        <v>613</v>
+      </c>
       <c r="F11" s="8"/>
       <c r="G11" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=10
+[Content=
+Do you expect something to block me?[Wait=500] Why would you ask me that?[Wait=500][Space=2]
+]
 ]</v>
       </c>
     </row>
@@ -15415,11 +15735,18 @@
       <c r="B12" s="6"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
-      <c r="E12" s="8"/>
+      <c r="E12" s="8" t="s">
+        <v>614</v>
+      </c>
       <c r="F12" s="8"/>
       <c r="G12" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=11
+[Content=
+I got myself a smart one, uh?[Wait=500][Space=2]
+I'm being conditional, cause there's a fence surrounding the entrance.[Wait=500][Space=2]
+Either have to get around or through it.[Wait=500][Space=2]
+]
 ]</v>
       </c>
     </row>
@@ -15430,11 +15757,20 @@
       <c r="B13" s="6"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
-      <c r="E13" s="8"/>
+      <c r="E13" s="8" t="s">
+        <v>641</v>
+      </c>
       <c r="F13" s="8"/>
       <c r="G13" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=12
+[Content=
+Oh-[Wait=500] Yeah...[Wait=500][Space=2]
+...[Wait=500][Space=2]
+I expected to feel better with someone else on the other end of the phone...[Wait=500] But I-...[Wait=500][Space=2]
+You know...[Wait=500] It's hard...[Wait=500][Space=2]
+[Color=Gray]*Footsteps*[Color=White]...[Wait=500][Space=2]
+]
 ]</v>
       </c>
     </row>
@@ -15445,11 +15781,18 @@
       <c r="B14" s="6"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
-      <c r="E14" s="8"/>
+      <c r="E14" s="8" t="s">
+        <v>615</v>
+      </c>
       <c r="F14" s="8"/>
       <c r="G14" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=13
+[Content=
+I-[Wait=500] I get it.[Wait=500][Space=2]
+It's good you're able to put yourself in my place a bit.[Wait=500] Thanks for acknowledging it.[Wait=500][Space=2]
+I'm starting to feel a bit more hopeful about getting out of here if you're on my side.[Wait=500][Space=2]
+]
 ]</v>
       </c>
     </row>
@@ -15460,11 +15803,20 @@
       <c r="B15" s="6"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
-      <c r="E15" s="8"/>
+      <c r="E15" s="8" t="s">
+        <v>616</v>
+      </c>
       <c r="F15" s="8"/>
       <c r="G15" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=14
+[Content=
+I'm getting there.[Wait=500] But I can already see the place's protected by a fence.[Wait=500][Space=2]
+It isn't a big deal, I could probably find another entrance.[Wait=500][Space=2]
+[Color=Gray]*Footsteps*[Color=White]...[Wait=500][Space=2]
+The metal looks brittle. I probably could bend it down and get over it.[Wait=500][Space=2]
+What do you think?[Wait=500][Space=2]
+]
 ]</v>
       </c>
     </row>
@@ -15475,11 +15827,18 @@
       <c r="B16" s="6"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
-      <c r="E16" s="8"/>
+      <c r="E16" s="8" t="s">
+        <v>617</v>
+      </c>
       <c r="F16" s="8"/>
       <c r="G16" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=15
+[Content=
+Hm-[Wait=500] Anyways, there's a fence blocking the way to the main entrance.[Wait=500][Space=2]
+I can either try and get through or go around.[Wait=500][Space=2]
+It looks weak enough to be bent, but this kind of buildings tend to have backdoors.[Wait=500][Space=2]
+]
 ]</v>
       </c>
     </row>
@@ -15490,11 +15849,18 @@
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
-      <c r="E17" s="8"/>
+      <c r="E17" s="8" t="s">
+        <v>618</v>
+      </c>
       <c r="F17" s="8"/>
       <c r="G17" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=16
+[Content=
+Yeah. The main entrance might be trapped, I'd rather find another way.[Wait=500][Space=2]
+[Color=Gray]*Footsteps*[Color=White]...[Wait=500][Space=2]
+Thinking outside the box might be the way to avoid some of the-[Wait=500] psycho keeping me here.[Wait=500][Space=2]
+]
 ]</v>
       </c>
     </row>
@@ -15505,11 +15871,19 @@
       <c r="B18" s="6"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
-      <c r="E18" s="8"/>
+      <c r="E18" s="8" t="s">
+        <v>619</v>
+      </c>
       <c r="F18" s="8"/>
       <c r="G18" s="23" t="str">
-        <f t="shared" si="0"/>
+        <f>"[Scene=" &amp; A18 &amp; IF(OR(B18&lt;&gt;"",C18&lt;&gt;"",D18&lt;&gt;""),CHAR(10),"") &amp; IF(B18&lt;&gt;"","[BeepBack=" &amp; B18 &amp; "]","") &amp; IF(C18&lt;&gt;"","[Connection=" &amp; C18 &amp; "]","") &amp; IF(D18&lt;&gt;"","[Timer=" &amp; D18 &amp; "]","") &amp; IF(E19&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp; E19 &amp; CHAR(10) &amp; "]","") &amp; IF(F18&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F18 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
         <v>[Scene=17
+[Content=
+...[Wait=500] No need to make me doubt...[Wait=500][Space=2]
+If that bastard really wants me to die I'm screwed anyways. Might as well minimize the risk.[Wait=500][Space=2]
+...[Wait=500][Space=2]
+Who knows...[Wait=500] He might be an idiot.[Wait=500][Space=2]
+]
 ]</v>
       </c>
     </row>
@@ -15520,12 +15894,13 @@
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
-      <c r="E19" s="8"/>
+      <c r="E19" s="8" t="s">
+        <v>620</v>
+      </c>
       <c r="F19" s="8"/>
-      <c r="G19" s="23" t="str">
-        <f t="shared" si="0"/>
-        <v>[Scene=18
-]</v>
+      <c r="G19" s="23" t="e">
+        <f>"[Scene=" &amp; A19 &amp; IF(OR(B19&lt;&gt;"",C19&lt;&gt;"",D19&lt;&gt;""),CHAR(10),"") &amp; IF(B19&lt;&gt;"","[BeepBack=" &amp; B19 &amp; "]","") &amp; IF(C19&lt;&gt;"","[Connection=" &amp; C19 &amp; "]","") &amp; IF(D19&lt;&gt;"","[Timer=" &amp; D19 &amp; "]","") &amp; IF(#REF!&lt;&gt;"",CHAR(10) &amp; "[Content=" &amp; CHAR(10) &amp;#REF! &amp; CHAR(10) &amp; "]","") &amp; IF(F19&lt;&gt;"",CHAR(10) &amp; "[Choices=" &amp; CHAR(10) &amp; F19 &amp; CHAR(10) &amp; "]","") &amp; CHAR(10) &amp; "]"</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="400.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -15535,11 +15910,22 @@
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
-      <c r="E20" s="8"/>
+      <c r="E20" s="8" t="s">
+        <v>621</v>
+      </c>
       <c r="F20" s="8"/>
       <c r="G20" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=19
+[Content=
+Talking about the zoo, guess what.[Wait=500] It's awfully close to this place.[Wait=500][Space=2]
+I can see the inside of the enclosures from there.[Wait=500][Space=2]
+Whoever designed this city should be fired.[Wait=500] Or even set on fire.[Wait=500][Space=2]
+Because I'm stuck inside their shittily designed city.[Wait=500][Space=2]
+That prick.[Wait=500][Space=2]
+[Color=Magenta][Beep=True][Color=Gray]*Distorted chuckle*[Color=White]...[Wait=500][Space=2]
+[Color=Magenta][Beep=True]YoU'[Wait=500][Beep=True]rE bEt[Wait=500][Beep=True]tEr hErE[Wait=500][Beep=True]  wItH mE[Wait=500][Beep=True]  tHaN aLo[Wait=500][Beep=True]nE iN[Wait=500][Beep=True]  tHe zOo.[Color=White][Wait=500][Space=2]
+]
 ]</v>
       </c>
     </row>
@@ -15550,11 +15936,19 @@
       <c r="B21" s="6"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
-      <c r="E21" s="8"/>
+      <c r="E21" s="8" t="s">
+        <v>622</v>
+      </c>
       <c r="F21" s="8"/>
       <c r="G21" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=20
+[Content=
+Wouldn't be trying to defend them, would we?[Wait=500][Space=2]
+Errm-[Wait=500] Anyways.[Wait=500][Space=2]
+Didn't realize the zoo was that close to the factory before.[Wait=500] Civil engineering failed some.[Wait=500][Space=2]
+[Color=Magenta][Beep=True]DaN[Wait=500][Beep=True]gErOuS[Wait=500][Beep=True]  pLa[Wait=500][Beep=True]cE.[Wait=500][Beep=True]  ExpEr[Wait=500][Beep=True]iMeNtS.[Color=White][Wait=500][Space=2]
+]
 ]</v>
       </c>
     </row>
@@ -15565,11 +15959,19 @@
       <c r="B22" s="6"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
-      <c r="E22" s="8"/>
+      <c r="E22" s="8" t="s">
+        <v>623</v>
+      </c>
       <c r="F22" s="8"/>
       <c r="G22" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=21
+[Content=
+Empty drums, debris, nothing but the usual shit.[Wait=500][Space=2]
+Nowhere else to go, you see, so for now I'll keep looking.[Wait=500][Space=2]
+Stressed out and hungry I feel, still haven't got anything to eat.[Wait=500][Space=2]
+I could really use oat meal, or anything that would get me going.[Wait=500][Space=2]
+]
 ]</v>
       </c>
     </row>
@@ -15580,11 +15982,21 @@
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
-      <c r="E23" s="8"/>
+      <c r="E23" s="8" t="s">
+        <v>624</v>
+      </c>
       <c r="F23" s="8"/>
       <c r="G23" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=22
+[Content=
+You're-...[Wait=500][Space=2]
+There's something written on the wall.[Wait=500][Space=2]
+...[Wait=500][Space=2]
+Please don't be scary.[Wait=500][Space=2]
+...[Wait=500][Space=2]
+Oh god.[Wait=500][Space=2]
+]
 ]</v>
       </c>
     </row>
@@ -15595,11 +16007,21 @@
       <c r="B24" s="6"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
-      <c r="E24" s="8"/>
+      <c r="E24" s="8" t="s">
+        <v>625</v>
+      </c>
       <c r="F24" s="8"/>
       <c r="G24" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=23
+[Content=
+M-[Wait=500] Me?[Wait=500] As I've said before I-...[Wait=500][Space=2]
+[Color=Magenta][Beep=True]OnE[Wait=500][Beep=True]  oF tHe[Wait=500][Beep=True]  pReVi[Wait=500][Beep=True]oUs.[Color=White][Wait=500] [Color=Gray]*Static*[Color=White]...[Wait=500][Space=2]
+[Color=Magenta][Beep=True]I'M[Wait=500][Beep=True]  hErE tO[Wait=500][Beep=True]  hElP yOu[Wait=500][Beep=True].  I'M aBlE[Wait=500][Beep=True]  tO cOmMu[Wait=500][Beep=True]nIcAtE tHrOuGh[Wait=500][Beep=True]  tHe dEsA[Wait=500][Beep=True]fEcTeD cOnTrOl.[Color=White][Wait=500][Space=2]
+[Color=Gray]*Static*[Color=White]...[Wait=500][Space=2]
+[Color=Magenta][Beep=True]SuR[Wait=500]viVoR[Wait=500][Beep=True],  i’M tRy[Wait=500][Beep=True]iNg tO gEt[Wait=500][Beep=True]  oThErS oUt[Wait=500][Beep=True]  oF hIs[Wait=500][Beep=True]  tRaPs.[Color=White][Wait=500][Space=2]
+Once again, I do NOT know why I'm here nor about any kind of experiments, just help me, alright?[Wait=500][Space=2]
+]
 ]</v>
       </c>
     </row>
@@ -15610,11 +16032,17 @@
       <c r="B25" s="6"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
-      <c r="E25" s="8"/>
+      <c r="E25" s="8" t="s">
+        <v>626</v>
+      </c>
       <c r="F25" s="8"/>
       <c r="G25" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=24
+[Content=
+What?[Wait=500] Who are you talking to?[Wait=500] You're really starting to freak me out.[Wait=500][Space=2]
+[Color=Magenta][Beep=True]CaN[Wait=500][Beep=True]’t sAy[Wait=500][Beep=True]  mOrE[Wait=500][Beep=True].  cOnNeC[Wait=500][Beep=True]tIoN  uNsTa[Wait=500][Beep=True]bLe[Wait=500][Beep=True].  yOu’Ll[Wait=500][Beep=True]  gEt cLo[Wait=500][Beep=True]sEr.[Color=White][Wait=500][Space=2]
+]
 ]</v>
       </c>
     </row>
@@ -15625,11 +16053,20 @@
       <c r="B26" s="6"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
-      <c r="E26" s="8"/>
+      <c r="E26" s="8" t="s">
+        <v>627</v>
+      </c>
       <c r="F26" s="8"/>
       <c r="G26" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=25
+[Content=
+Of course I'm going to worry!!![Wait=500][Space=2]
+You're giving me no explanation after saying shit about some experiment. Are there more people with you?[Wait=500][Space=2]
+...[Wait=500][Space=2]
+You're always alternating between reinsuring and cryptic, talking to the fucking voices now![Wait=500][Space=2]
+Am-[Wait=500] Am I a game to you?[Wait=500] Are you going to fucking tell?![Wait=500][Space=2]
+]
 ]</v>
       </c>
     </row>
@@ -15640,11 +16077,21 @@
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
-      <c r="E27" s="8"/>
+      <c r="E27" s="8" t="s">
+        <v>628</v>
+      </c>
       <c r="F27" s="8"/>
       <c r="G27" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=26
+[Content=
+And...[Wait=500] You're just gonna say that now?[Wait=500][Space=2]
+Uh...[Wait=500] Nevermind. I'm not even gonna ask anymore.[Wait=500][Space=2]
+.[Wait=500].[Wait=500].[Wait=500][Space=2]
+But should we reaaally trust them?[Wait=500][Space=2]
+I mean, why would anyone other than the person behind all of this try to talk to you.[Wait=500][Space=2]
+And why can't I hear them?[Wait=500][Space=2]
+]
 ]</v>
       </c>
     </row>
@@ -15655,11 +16102,21 @@
       <c r="B28" s="6"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
-      <c r="E28" s="8"/>
+      <c r="E28" s="8" t="s">
+        <v>629</v>
+      </c>
       <c r="F28" s="8"/>
       <c r="G28" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=27
+[Content=
+Which means...[Wait=500] They're on the island.[Wait=500][Space=2]
+Great.[Wait=500][Space=2]
+That either means a helping hand... or extra danger.[Wait=500][Space=2]
+As if all of this needed more complexity.[Wait=500][Space=2]
+So they're going to help you guide me if I understood well.[Wait=500][Space=2]
+Doesn't sound like a trap.[Wait=500][Space=2]
+]
 ]</v>
       </c>
     </row>
@@ -15670,11 +16127,18 @@
       <c r="B29" s="6"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
-      <c r="E29" s="8"/>
+      <c r="E29" s="8" t="s">
+        <v>630</v>
+      </c>
       <c r="F29" s="8"/>
       <c r="G29" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=28
+[Content=
+Yeah...[Wait=500] I know.[Wait=500][Space=2]
+Let's just think positively![Wait=500] Everything's...[Wait=500] Fine.[Wait=500][Space=2]
+New hope.[Wait=500] Island friend.[Wait=500] Good news aaall around.[Wait=500][Space=2]
+]
 ]</v>
       </c>
     </row>
@@ -15685,11 +16149,18 @@
       <c r="B30" s="6"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
-      <c r="E30" s="8"/>
+      <c r="E30" s="8" t="s">
+        <v>631</v>
+      </c>
       <c r="F30" s="8"/>
       <c r="G30" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=29
+[Content=
+Uuh-[Wait=500] Sure...[Wait=500][Space=2]
+...[Wait=500][Space=2]
+I'll-...[Wait=500][Space=2]
+]
 ]</v>
       </c>
     </row>
@@ -15700,11 +16171,22 @@
       <c r="B31" s="6"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
-      <c r="E31" s="8"/>
+      <c r="E31" s="8" t="s">
+        <v>632</v>
+      </c>
       <c r="F31" s="8"/>
       <c r="G31" s="23" t="str">
         <f t="shared" si="0"/>
         <v>[Scene=30
+[Content=
+Of course.[Wait=500][Space=2]
+Let's just start m-...[Wait=500][Space=2]
+...[Wait=500][Space=2]
+Writings.[Wait=500][Space=2]
+Writings on the wall.[Wait=500] Please.[Wait=500] Why?[Wait=500][Space=2]
+Oh no, don't tell me these are creepy letters-...[Wait=500][Space=2]
+On the wall.[Wait=500] I'm so sick.[Wait=500][Space=2]
+]
 ]</v>
       </c>
     </row>

</xml_diff>